<commit_message>
Formula for Total Number of Events.
</commit_message>
<xml_diff>
--- a/OtAoFPA Program Data.xlsx
+++ b/OtAoFPA Program Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rishi\Documents\Python\OtAoFPA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F039CC10-91AE-48DD-838C-63B1289AC83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B701C135-B11E-48DC-8610-C83A238DA8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B82B5DA4-62A4-4ADF-8494-925F1F855B7B}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="10">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
     <numFmt numFmtId="166" formatCode="0.00000000000"/>
@@ -96,7 +96,8 @@
     <numFmt numFmtId="170" formatCode="0.000000000000000"/>
     <numFmt numFmtId="171" formatCode="0.0000000000000000"/>
     <numFmt numFmtId="172" formatCode="0.00000000000000000"/>
-    <numFmt numFmtId="178" formatCode="0.0000000000"/>
+    <numFmt numFmtId="173" formatCode="0.0000000000"/>
+    <numFmt numFmtId="174" formatCode="0.000000000000000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -358,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -394,9 +395,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -441,7 +439,7 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -451,6 +449,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -573,6 +580,50 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="#,##0.000000000000000" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$9</c:f>
@@ -613,22 +664,19 @@
                   <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16384</c:v>
+                  <c:v>12288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>294912</c:v>
+                  <c:v>196608</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4194304</c:v>
+                  <c:v>2621440</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52428800</c:v>
+                  <c:v>31457280</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>603979776</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6576668672</c:v>
+                  <c:v>352321536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -641,7 +689,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1054,22 +1101,19 @@
                   <c:v>0.4296875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.50390625</c:v>
+                  <c:v>0.423828125</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000000000000000">
-                  <c:v>0.55914984809027701</c:v>
+                  <c:v>0.42228190104166602</c:v>
                 </c:pt>
-                <c:pt idx="3" formatCode="0.000000000000000">
-                  <c:v>0.59364795684814398</c:v>
+                <c:pt idx="3" formatCode="0.00000000000000">
+                  <c:v>0.42391357421874998</c:v>
                 </c:pt>
-                <c:pt idx="4" formatCode="0.00000000000000">
-                  <c:v>0.61715705871582005</c:v>
+                <c:pt idx="4" formatCode="0.000000000000000">
+                  <c:v>0.42726440429687501</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.000000000000000">
-                  <c:v>0.634345908959706</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="0.000000000000000">
-                  <c:v>0.64754875399628398</c:v>
+                  <c:v>0.431336539132254</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,7 +1126,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1517,9 +1560,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:delete val="1"/>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$9</c:f>
@@ -1556,26 +1596,26 @@
               <c:numCache>
                 <c:formatCode>0.0000000000000000</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="0.00000000000000000">
-                  <c:v>1.0481675465901636E-3</c:v>
+                <c:pt idx="0" formatCode="0.000000000000000000">
+                  <c:v>8.8342030843098669E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4365434646606398E-2</c:v>
+                  <c:v>1.11456712086995E-2</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.000000000000000">
-                  <c:v>0.25243751207987403</c:v>
+                  <c:v>0.16654833157857232</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="0.00000000000000">
-                  <c:v>3.5716193517049102</c:v>
+                  <c:v>2.3161095778147298</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="0.0000000000000">
-                  <c:v>45.096443414688075</c:v>
+                  <c:v>26.510492881139069</c:v>
                 </c:pt>
-                <c:pt idx="5" formatCode="0.00000000000">
-                  <c:v>568.20172047614994</c:v>
+                <c:pt idx="5" formatCode="0.000000000000">
+                  <c:v>331.76863423983201</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="0.00000000000">
-                  <c:v>6221.8755907217637</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,7 +1894,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00000000000000000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000000000000000000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4047,8 +4087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBDC94D5-E8E0-480C-903D-03926A1CC3FA}">
   <dimension ref="B1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="121" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4066,10 +4106,10 @@
       <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -4092,197 +4132,185 @@
       <c r="B3" s="10">
         <v>3</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>512</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="21">
         <v>220</v>
       </c>
       <c r="E3" s="11">
         <v>0.4296875</v>
       </c>
       <c r="F3" s="12">
-        <v>1.06310844421386E-3</v>
-      </c>
-      <c r="G3" s="12">
-        <v>1.01065635681152E-3</v>
-      </c>
-      <c r="H3" s="12">
-        <v>1.07073783874511E-3</v>
-      </c>
-      <c r="I3" s="13">
+        <v>1.6307830810546799E-3</v>
+      </c>
+      <c r="G3" s="31">
+        <v>5.07116317749023E-4</v>
+      </c>
+      <c r="H3" s="31">
+        <v>5.1236152648925705E-4</v>
+      </c>
+      <c r="I3" s="32">
         <f>(F3+G3+H3)/3</f>
-        <v>1.0481675465901636E-3</v>
+        <v>8.8342030843098669E-4</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>4</v>
       </c>
-      <c r="C4" s="23">
-        <v>16384</v>
-      </c>
-      <c r="D4" s="23">
-        <v>8256</v>
-      </c>
-      <c r="E4" s="15">
-        <v>0.50390625</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1.50215625762939E-2</v>
-      </c>
-      <c r="G4" s="16">
-        <v>1.39110088348388E-2</v>
-      </c>
-      <c r="H4" s="16">
-        <v>1.4163732528686499E-2</v>
-      </c>
-      <c r="I4" s="18">
+      <c r="C4" s="22">
+        <v>12288</v>
+      </c>
+      <c r="D4" s="22">
+        <v>5208</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.423828125</v>
+      </c>
+      <c r="F4" s="15">
+        <v>1.16541385650634E-2</v>
+      </c>
+      <c r="G4" s="15">
+        <v>1.11699104309082E-2</v>
+      </c>
+      <c r="H4" s="15">
+        <v>1.0612964630126899E-2</v>
+      </c>
+      <c r="I4" s="17">
         <f t="shared" ref="I4:I10" si="0">(F4+G4+H4)/3</f>
-        <v>1.4365434646606398E-2</v>
+        <v>1.11456712086995E-2</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>5</v>
       </c>
-      <c r="C5" s="23">
-        <v>294912</v>
-      </c>
-      <c r="D5" s="23">
-        <v>164900</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0.55914984809027701</v>
-      </c>
-      <c r="F5" s="17">
-        <v>0.25121331214904702</v>
-      </c>
-      <c r="G5" s="17">
-        <v>0.25249028205871499</v>
-      </c>
-      <c r="H5" s="20">
-        <v>0.25360894203186002</v>
-      </c>
-      <c r="I5" s="19">
+      <c r="C5" s="22">
+        <v>196608</v>
+      </c>
+      <c r="D5" s="22">
+        <v>83024</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.42228190104166602</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.16847181320190399</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0.16394782066345201</v>
+      </c>
+      <c r="H5" s="16">
+        <v>0.167225360870361</v>
+      </c>
+      <c r="I5" s="18">
         <f t="shared" si="0"/>
-        <v>0.25243751207987403</v>
+        <v>0.16654833157857232</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+      <c r="B6" s="13">
         <v>6</v>
       </c>
-      <c r="C6" s="23">
-        <v>4194304</v>
-      </c>
-      <c r="D6" s="23">
-        <v>2489940</v>
-      </c>
-      <c r="E6" s="17">
-        <v>0.59364795684814398</v>
-      </c>
-      <c r="F6" s="20">
-        <v>3.5567932128906201</v>
-      </c>
-      <c r="G6" s="26">
-        <v>3.5879042148589999</v>
-      </c>
-      <c r="H6" s="20">
-        <v>3.5701606273651101</v>
-      </c>
-      <c r="I6" s="29">
+      <c r="C6" s="22">
+        <v>2621440</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1111264</v>
+      </c>
+      <c r="E6" s="19">
+        <v>0.42391357421874998</v>
+      </c>
+      <c r="F6" s="19">
+        <v>2.2640810012817298</v>
+      </c>
+      <c r="G6" s="19">
+        <v>2.32328748703002</v>
+      </c>
+      <c r="H6" s="19">
+        <v>2.3609602451324401</v>
+      </c>
+      <c r="I6" s="28">
         <f t="shared" si="0"/>
-        <v>3.5716193517049102</v>
+        <v>2.3161095778147298</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>7</v>
       </c>
-      <c r="C7" s="23">
-        <v>52428800</v>
-      </c>
-      <c r="D7" s="23">
-        <v>32356804</v>
-      </c>
-      <c r="E7" s="20">
-        <v>0.61715705871582005</v>
-      </c>
-      <c r="F7" s="27">
-        <v>44.305991172790499</v>
-      </c>
-      <c r="G7" s="27">
-        <v>45.824229717254603</v>
-      </c>
-      <c r="H7" s="27">
-        <v>45.159109354019101</v>
-      </c>
-      <c r="I7" s="30">
+      <c r="C7" s="22">
+        <v>31457280</v>
+      </c>
+      <c r="D7" s="22">
+        <v>13440576</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.42726440429687501</v>
+      </c>
+      <c r="F7" s="26">
+        <v>26.398905515670702</v>
+      </c>
+      <c r="G7" s="26">
+        <v>26.694002389907801</v>
+      </c>
+      <c r="H7" s="26">
+        <v>26.438570737838699</v>
+      </c>
+      <c r="I7" s="29">
         <f t="shared" si="0"/>
-        <v>45.096443414688075</v>
+        <v>26.510492881139069</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>8</v>
       </c>
-      <c r="C8" s="23">
-        <v>603979776</v>
-      </c>
-      <c r="D8" s="23">
-        <v>383132100</v>
-      </c>
-      <c r="E8" s="17">
-        <v>0.634345908959706</v>
-      </c>
-      <c r="F8" s="26">
-        <v>568.42039251327503</v>
-      </c>
-      <c r="G8" s="26">
-        <v>571.78876757621697</v>
-      </c>
-      <c r="H8" s="26">
-        <v>564.39600133895794</v>
-      </c>
-      <c r="I8" s="31">
+      <c r="C8" s="22">
+        <v>352321536</v>
+      </c>
+      <c r="D8" s="22">
+        <v>151969152</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.431336539132254</v>
+      </c>
+      <c r="F8" s="25">
+        <v>329.74270033836302</v>
+      </c>
+      <c r="G8" s="24">
+        <v>332.94395828247002</v>
+      </c>
+      <c r="H8" s="25">
+        <v>332.61924409866299</v>
+      </c>
+      <c r="I8" s="33">
         <f t="shared" si="0"/>
-        <v>568.20172047614994</v>
+        <v>331.76863423983201</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>9</v>
       </c>
-      <c r="C9" s="23">
-        <v>6576668672</v>
-      </c>
-      <c r="D9" s="23">
-        <v>4258713604</v>
-      </c>
-      <c r="E9" s="17">
-        <v>0.64754875399628398</v>
-      </c>
-      <c r="F9" s="25">
-        <v>6204.3940157890302</v>
-      </c>
-      <c r="G9" s="28">
-        <v>6226.9129178523999</v>
-      </c>
-      <c r="H9" s="25">
-        <v>6234.3198385238602</v>
-      </c>
-      <c r="I9" s="31">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="30">
         <f t="shared" si="0"/>
-        <v>6221.8755907217637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>10</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="6"/>

</xml_diff>